<commit_message>
Added Hands On Demos - Day 2
</commit_message>
<xml_diff>
--- a/Microservices-Spring TOC.xlsx
+++ b/Microservices-Spring TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="1"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -723,7 +723,7 @@
     <t>9. Summary</t>
   </si>
   <si>
-    <t>Hands On Lab 1 - Spring MVC With Data JPA</t>
+    <t>Hands On Lab 1 - Spring Data REST - Developing RESTful APIs with Ease</t>
   </si>
   <si>
     <t>Day 7</t>
@@ -1078,8 +1078,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="39">
     <font>
@@ -1215,9 +1215,30 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1233,29 +1254,15 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1274,13 +1281,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1315,8 +1315,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1330,7 +1331,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1340,20 +1354,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1392,13 +1392,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1410,43 +1446,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1464,7 +1464,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1476,25 +1476,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1506,7 +1512,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1524,19 +1548,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1548,31 +1560,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1653,17 +1653,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1675,6 +1664,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1703,15 +1707,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1727,17 +1722,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1750,18 +1741,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1771,31 +1771,31 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1807,94 +1807,94 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2323,7 +2323,7 @@
   <sheetPr/>
   <dimension ref="A7:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -2524,7 +2524,7 @@
   <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
     </sheetView>
@@ -3068,7 +3068,7 @@
   <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
     </sheetView>
@@ -3562,7 +3562,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C23" sqref="C23:C24"/>
     </sheetView>
@@ -3778,7 +3778,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
@@ -3998,10 +3998,10 @@
   <sheetPr/>
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -4519,7 +4519,7 @@
   <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
     </sheetView>

</xml_diff>

<commit_message>
Added Hands On Demo - Day 8
</commit_message>
<xml_diff>
--- a/Microservices-Spring TOC.xlsx
+++ b/Microservices-Spring TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="3" activeTab="3"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -459,6 +459,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Spring REST is the way to go for Java server applications combined with Angular, React, Android or iOS client apps.                </t>
     </r>
     <r>
@@ -798,7 +806,7 @@
     <t>12. Summary</t>
   </si>
   <si>
-    <t>Hands On Lab 1 - Expose RESTful APIs around Spring Data Repositories</t>
+    <t>Hands On Lab 2 - Expose RESTful APIs around Spring Data Repositories</t>
   </si>
   <si>
     <t>Day 8</t>
@@ -1076,10 +1084,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="39">
     <font>
@@ -1216,7 +1224,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1237,17 +1260,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1256,6 +1270,22 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1284,13 +1314,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -1299,16 +1322,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1322,24 +1345,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1352,8 +1359,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1392,7 +1400,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1404,37 +1460,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1446,19 +1478,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1476,13 +1496,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1494,7 +1538,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1506,19 +1550,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1530,19 +1568,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1554,25 +1580,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1653,6 +1661,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1664,15 +1696,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1718,6 +1741,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1726,42 +1758,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1771,134 +1779,134 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1935,6 +1943,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2337,174 +2348,174 @@
   <sheetData>
     <row r="7" ht="13.5"/>
     <row r="8" ht="13.5" spans="6:9">
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="29" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="6:9">
-      <c r="F9" s="29">
+      <c r="F9" s="30">
         <v>1</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="31">
+      <c r="H9" s="32">
         <v>2</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="32">
         <v>8</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="6:9">
-      <c r="F10" s="32">
+      <c r="F10" s="33">
         <v>2</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="31">
+      <c r="H10" s="32">
         <v>1</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="32">
         <v>4</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="6:9">
-      <c r="F11" s="34">
+      <c r="F11" s="35">
         <v>3</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="31">
+      <c r="H11" s="32">
         <v>1</v>
       </c>
-      <c r="I11" s="31">
+      <c r="I11" s="32">
         <v>4</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="6:9">
-      <c r="F12" s="32">
+      <c r="F12" s="33">
         <v>4</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="31">
+      <c r="H12" s="32">
         <v>1</v>
       </c>
-      <c r="I12" s="31">
+      <c r="I12" s="32">
         <v>4</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="6:9">
-      <c r="F13" s="34">
+      <c r="F13" s="35">
         <v>5</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="G13" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="31">
+      <c r="H13" s="32">
         <v>2</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="32">
         <v>8</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="6:9">
-      <c r="F14" s="32">
+      <c r="F14" s="33">
         <v>6</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="31">
+      <c r="H14" s="32">
         <v>2</v>
       </c>
-      <c r="I14" s="31">
+      <c r="I14" s="32">
         <v>8</v>
       </c>
     </row>
     <row r="15" ht="15.75" spans="6:9">
-      <c r="F15" s="32">
+      <c r="F15" s="33">
         <v>7</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="31">
+      <c r="H15" s="32">
         <v>1</v>
       </c>
-      <c r="I15" s="31">
+      <c r="I15" s="32">
         <v>4</v>
       </c>
     </row>
     <row r="16" ht="15.75" spans="6:9">
-      <c r="F16" s="35"/>
-      <c r="G16" s="36" t="s">
+      <c r="F16" s="36"/>
+      <c r="G16" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="37" t="s">
+      <c r="H16" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="37" t="s">
+      <c r="I16" s="38" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="24" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="38">
+      <c r="A22" s="39">
         <v>1</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="38">
+      <c r="A25" s="39">
         <v>2</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
     </row>
     <row r="26" spans="2:6">
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2778,7 +2789,7 @@
       <c r="B34" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="24" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2877,7 +2888,7 @@
       <c r="B48" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="C48" s="25" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2911,7 +2922,7 @@
     </row>
     <row r="53" ht="18" spans="1:3">
       <c r="A53" s="14"/>
-      <c r="B53" s="25"/>
+      <c r="B53" s="26"/>
       <c r="C53" s="5"/>
     </row>
     <row r="54" ht="15" spans="1:3">
@@ -2919,7 +2930,7 @@
       <c r="B54" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C54" s="24" t="s">
+      <c r="C54" s="25" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3009,7 +3020,7 @@
     </row>
     <row r="67" ht="15" spans="1:3">
       <c r="A67" s="14"/>
-      <c r="B67" s="26"/>
+      <c r="B67" s="27"/>
       <c r="C67" s="5"/>
     </row>
     <row r="68" ht="15" spans="1:3">
@@ -3218,7 +3229,7 @@
     <row r="19" ht="18.75" spans="1:3">
       <c r="A19" s="14"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="17"/>
+      <c r="C19" s="18"/>
     </row>
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="14"/>
@@ -3322,7 +3333,7 @@
     </row>
     <row r="34" ht="15" spans="1:3">
       <c r="A34" s="14"/>
-      <c r="B34" s="21"/>
+      <c r="B34" s="22"/>
       <c r="C34" s="15"/>
     </row>
     <row r="35" ht="15" spans="1:3">
@@ -3385,7 +3396,7 @@
     </row>
     <row r="43" ht="15" spans="1:3">
       <c r="A43" s="14"/>
-      <c r="B43" s="21"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="15"/>
     </row>
     <row r="44" ht="15" spans="1:3">
@@ -3420,7 +3431,7 @@
     </row>
     <row r="48" ht="15" spans="1:3">
       <c r="A48" s="14"/>
-      <c r="B48" s="21"/>
+      <c r="B48" s="22"/>
       <c r="C48" s="15"/>
     </row>
     <row r="49" ht="15" spans="1:3">
@@ -3561,8 +3572,8 @@
   <sheetPr/>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
@@ -3649,7 +3660,7 @@
     <row r="10" ht="18.75" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="17"/>
+      <c r="C10" s="18"/>
     </row>
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="3"/>
@@ -3704,7 +3715,7 @@
     </row>
     <row r="18" ht="15" spans="1:3">
       <c r="A18" s="3"/>
-      <c r="B18" s="21"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="15"/>
     </row>
     <row r="19" ht="15" spans="1:3">
@@ -3742,14 +3753,14 @@
     <row r="23" ht="20" customHeight="1" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="23" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="22"/>
+      <c r="C24" s="23"/>
     </row>
     <row r="25" ht="13" customHeight="1" spans="1:3">
       <c r="A25" s="3"/>
@@ -3758,17 +3769,17 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" ht="18.75" spans="1:3">
+    <row r="26" ht="15" spans="1:3">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="23" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="27" ht="18.75" spans="1:3">
+    <row r="27" ht="15" spans="1:3">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="23" t="s">
         <v>151</v>
       </c>
     </row>
@@ -3830,169 +3841,169 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="18.75" spans="1:3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>153</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" ht="15" spans="1:3">
-      <c r="A4" s="18"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
     <row r="5" ht="18.75" spans="1:3">
-      <c r="A5" s="18"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="18" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="6" ht="18.75" spans="1:3">
-      <c r="A6" s="18"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="18" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="7" ht="18.75" spans="1:3">
-      <c r="A7" s="18"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="18" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="8" ht="18.75" spans="1:3">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="18" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
     <row r="10" ht="18.75" spans="1:3">
-      <c r="A10" s="18"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="18" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="11" ht="18.75" spans="1:3">
-      <c r="A11" s="18"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="18" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="12" ht="37.5" spans="1:3">
-      <c r="A12" s="18"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="18" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="13" ht="18.75" spans="1:3">
-      <c r="A13" s="18"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="18" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="14" ht="37.5" spans="1:3">
-      <c r="A14" s="18"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="18" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="15" ht="18.75" spans="1:3">
-      <c r="A15" s="18"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="18" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="16" ht="37.5" spans="1:3">
-      <c r="A16" s="18"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="18" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="17" ht="18.75" spans="1:3">
-      <c r="A17" s="18"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="18" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="18" ht="37.5" spans="1:3">
-      <c r="A18" s="18"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="18" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="19" ht="18.75" spans="1:3">
-      <c r="A19" s="18"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="18" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="20" ht="18.75" spans="1:3">
-      <c r="A20" s="18"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="18" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="21" ht="18.75" spans="1:3">
-      <c r="A21" s="18"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="18" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="22" ht="18.75" spans="1:3">
-      <c r="A22" s="18"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="18" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="23" ht="18.75" spans="1:3">
-      <c r="A23" s="18"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="18" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="24" ht="18.75" spans="1:3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19" t="s">
+      <c r="A24" s="19"/>
+      <c r="B24" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="21" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="25" ht="37.5" spans="1:3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="17" t="s">
+      <c r="A25" s="19"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="18" t="s">
         <v>176</v>
       </c>
     </row>
@@ -4020,9 +4031,9 @@
   <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
+      <selection pane="bottomLeft" activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -4426,7 +4437,7 @@
     <row r="55" ht="15" spans="1:3">
       <c r="A55" s="12"/>
       <c r="B55" s="4"/>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="16" t="s">
         <v>224</v>
       </c>
     </row>
@@ -4539,10 +4550,10 @@
   <sheetPr/>
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="3"/>
@@ -5002,11 +5013,12 @@
       <c r="D72" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="A3:A34"/>
     <mergeCell ref="A37:A60"/>
+    <mergeCell ref="A61:A62"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B15:B22"/>
@@ -5029,7 +5041,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>

</xml_diff>

<commit_message>
Added Course Materials - Day 9 and 10.
</commit_message>
<xml_diff>
--- a/Microservices-Spring TOC.xlsx
+++ b/Microservices-Spring TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="4" activeTab="6"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="301">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -927,9 +927,6 @@
     <t>9. Wrap-up</t>
   </si>
   <si>
-    <t>Hands On Lab 1 - Add a security filter in Spring Boot</t>
-  </si>
-  <si>
     <t>Day 9</t>
   </si>
   <si>
@@ -999,21 +996,10 @@
     <t>5. What Next?</t>
   </si>
   <si>
-    <t>Hands On Lab 1 - Spring Security with JWT for REST API</t>
-  </si>
-  <si>
     <t>Day 10</t>
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">Spring Boot and Angular have forever changed how web applications are built. Learn how to work with both of these technologies and how to integrate them together.                                              </t>
     </r>
     <r>
@@ -1024,20 +1010,34 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Expose endpoint using Spring Boot.                                            Consume this endpoint using  Angular and display the data.</t>
+      <t>Expose endpoint using Spring Boot.                                            Consume this endpoint using  Angular and display the data</t>
     </r>
-  </si>
-  <si>
-    <t>1. Developing the backend with Spring MVC</t>
-  </si>
-  <si>
-    <t>2. Project Architecture</t>
-  </si>
-  <si>
-    <t>3. Directory Structure</t>
-  </si>
-  <si>
-    <t>4. Demo:Create the Employee model class</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>2. Developing the backend with Spring MVC</t>
+  </si>
+  <si>
+    <t>1.The Spring Boot Application</t>
+  </si>
+  <si>
+    <t>2. The Maven Dependencies</t>
+  </si>
+  <si>
+    <t>3.The JPA Entity Class</t>
+  </si>
+  <si>
+    <t>4. The UserRepository Interface</t>
   </si>
   <si>
     <t>5. Demo:Create the REST Controller</t>
@@ -1046,37 +1046,49 @@
     <t>6. Demo:Enable CORS</t>
   </si>
   <si>
-    <t>7. Demo:Run the Application</t>
-  </si>
-  <si>
-    <t>2. Developing the frontend with Angular</t>
-  </si>
-  <si>
-    <t>2. Install node js</t>
-  </si>
-  <si>
-    <t>3. Install Angular CLI</t>
-  </si>
-  <si>
-    <t>4. Demo:Generating an Angular app</t>
-  </si>
-  <si>
-    <t>5. Demo:Generating the employee component</t>
-  </si>
-  <si>
-    <t>6. Demo:Configure routing</t>
-  </si>
-  <si>
-    <t>7. Demo:Create HttpClient Service</t>
-  </si>
-  <si>
-    <t>8. Demo:Insert HttpClient Service in Employee Component</t>
-  </si>
-  <si>
-    <t>9. Demo:Run the Application</t>
-  </si>
-  <si>
-    <t>Hands On Lab 1 - Building a Web Application with Spring Boot and Angular</t>
+    <t>7. Demo: Bootstrapping the Spring Boot Application</t>
+  </si>
+  <si>
+    <t>3. Developing the frontend with Angular</t>
+  </si>
+  <si>
+    <t>1. The Angular Application</t>
+  </si>
+  <si>
+    <t>2.Angular CLI Installation</t>
+  </si>
+  <si>
+    <t>3. Project Scaffolding With Angular CLI</t>
+  </si>
+  <si>
+    <t>4.  The Angular Application's Entry Point</t>
+  </si>
+  <si>
+    <t>5. The app.component.ts Root Component</t>
+  </si>
+  <si>
+    <t>6. The app.component.html File</t>
+  </si>
+  <si>
+    <t>7. The User Class</t>
+  </si>
+  <si>
+    <t>8. The UserService Service</t>
+  </si>
+  <si>
+    <t>9. The UserListComponent Component</t>
+  </si>
+  <si>
+    <t>10. The UserFormComponent Component</t>
+  </si>
+  <si>
+    <t>11. The app-routing.module.ts File</t>
+  </si>
+  <si>
+    <t>12. The app.module.ts File</t>
+  </si>
+  <si>
+    <t>13.  Running the Application</t>
   </si>
 </sst>
 </file>
@@ -1084,10 +1096,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="39">
     <font>
@@ -1141,14 +1153,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1163,6 +1167,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1224,22 +1236,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1252,6 +1249,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -1260,8 +1265,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1269,23 +1275,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1308,6 +1298,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1322,6 +1319,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1330,23 +1335,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1362,6 +1352,28 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1400,13 +1412,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1418,67 +1442,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1496,19 +1484,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1520,25 +1550,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1550,37 +1562,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1664,8 +1676,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1681,21 +1693,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1724,6 +1721,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1739,11 +1745,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1761,15 +1773,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1779,134 +1791,134 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1918,34 +1930,31 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1958,7 +1967,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2348,174 +2357,174 @@
   <sheetData>
     <row r="7" ht="13.5"/>
     <row r="8" ht="13.5" spans="6:9">
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="28" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="6:9">
-      <c r="F9" s="30">
+      <c r="F9" s="29">
         <v>1</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="31">
         <v>2</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="31">
         <v>8</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="6:9">
-      <c r="F10" s="33">
+      <c r="F10" s="32">
         <v>2</v>
       </c>
-      <c r="G10" s="34" t="s">
+      <c r="G10" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="31">
         <v>1</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="31">
         <v>4</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="6:9">
-      <c r="F11" s="35">
+      <c r="F11" s="34">
         <v>3</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="32">
+      <c r="H11" s="31">
         <v>1</v>
       </c>
-      <c r="I11" s="32">
+      <c r="I11" s="31">
         <v>4</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="6:9">
-      <c r="F12" s="33">
+      <c r="F12" s="32">
         <v>4</v>
       </c>
-      <c r="G12" s="34" t="s">
+      <c r="G12" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="31">
         <v>1</v>
       </c>
-      <c r="I12" s="32">
+      <c r="I12" s="31">
         <v>4</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="6:9">
-      <c r="F13" s="35">
+      <c r="F13" s="34">
         <v>5</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="31">
         <v>2</v>
       </c>
-      <c r="I13" s="32">
+      <c r="I13" s="31">
         <v>8</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="6:9">
-      <c r="F14" s="33">
+      <c r="F14" s="32">
         <v>6</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="G14" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="32">
+      <c r="H14" s="31">
         <v>2</v>
       </c>
-      <c r="I14" s="32">
+      <c r="I14" s="31">
         <v>8</v>
       </c>
     </row>
     <row r="15" ht="15.75" spans="6:9">
-      <c r="F15" s="33">
+      <c r="F15" s="32">
         <v>7</v>
       </c>
-      <c r="G15" s="34" t="s">
+      <c r="G15" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="31">
         <v>1</v>
       </c>
-      <c r="I15" s="32">
+      <c r="I15" s="31">
         <v>4</v>
       </c>
     </row>
     <row r="16" ht="15.75" spans="6:9">
-      <c r="F16" s="36"/>
-      <c r="G16" s="37" t="s">
+      <c r="F16" s="35"/>
+      <c r="G16" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="37" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="39">
+      <c r="A22" s="38">
         <v>1</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="39">
+      <c r="A25" s="38">
         <v>2</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
     </row>
     <row r="26" spans="2:6">
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2570,7 +2579,7 @@
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -2578,12 +2587,12 @@
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="5"/>
     </row>
     <row r="5" ht="15" spans="1:3">
-      <c r="A5" s="14"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
         <v>24</v>
       </c>
@@ -2592,47 +2601,47 @@
       </c>
     </row>
     <row r="6" ht="15" spans="1:3">
-      <c r="A6" s="14"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="6"/>
       <c r="C6" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
-      <c r="A7" s="14"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="6"/>
       <c r="C7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
-      <c r="A8" s="14"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="6"/>
       <c r="C8" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
-      <c r="A9" s="14"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
-      <c r="A10" s="14"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="6"/>
       <c r="C10" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:3">
-      <c r="A11" s="14"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
     </row>
     <row r="12" ht="15" spans="1:3">
-      <c r="A12" s="14"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="6" t="s">
         <v>31</v>
       </c>
@@ -2641,53 +2650,53 @@
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
-      <c r="A13" s="14"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
-      <c r="A14" s="14"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:3">
-      <c r="A15" s="14"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:3">
-      <c r="A16" s="14"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
-      <c r="A17" s="14"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
-      <c r="A18" s="14"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="14"/>
-      <c r="C19" s="15"/>
+      <c r="A19" s="12"/>
+      <c r="C19" s="13"/>
     </row>
     <row r="20" ht="15" spans="1:3">
-      <c r="A20" s="14"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="6" t="s">
         <v>38</v>
       </c>
@@ -2696,40 +2705,40 @@
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="6"/>
       <c r="C21" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
-      <c r="A22" s="14"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="6"/>
       <c r="C22" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
-      <c r="A23" s="14"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="6"/>
       <c r="C23" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:3">
-      <c r="A24" s="14"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="6"/>
       <c r="C24" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
-      <c r="A25" s="14"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
     <row r="26" ht="15" spans="1:3">
-      <c r="A26" s="14"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="6" t="s">
         <v>43</v>
       </c>
@@ -2738,93 +2747,93 @@
       </c>
     </row>
     <row r="27" ht="15" spans="1:3">
-      <c r="A27" s="14"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="6"/>
       <c r="C27" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" ht="15" spans="1:3">
-      <c r="A28" s="14"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="6"/>
       <c r="C28" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="29" ht="15" spans="1:3">
-      <c r="A29" s="14"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="6"/>
       <c r="C29" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:3">
-      <c r="A30" s="14"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="6"/>
       <c r="C30" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
-      <c r="A31" s="14"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="6"/>
       <c r="C31" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
-      <c r="A32" s="14"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="6"/>
       <c r="C32" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
-      <c r="A33" s="14"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="14"/>
-      <c r="B34" s="4" t="s">
+      <c r="A34" s="12"/>
+      <c r="B34" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="14"/>
-      <c r="B35" s="4"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="14"/>
       <c r="C35" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="4"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="14"/>
       <c r="C36" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="4"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="14"/>
       <c r="C37" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="14"/>
-      <c r="B38" s="4"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="14"/>
       <c r="C38" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" spans="1:3">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
     </row>
     <row r="40" ht="27" customHeight="1" spans="1:3">
       <c r="A40" s="2" t="s">
@@ -2834,7 +2843,7 @@
       <c r="C40" s="2"/>
     </row>
     <row r="41" ht="15" spans="1:3">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -2845,137 +2854,137 @@
       </c>
     </row>
     <row r="42" ht="15" spans="1:3">
-      <c r="A42" s="14"/>
+      <c r="A42" s="12"/>
       <c r="B42" s="6"/>
       <c r="C42" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
-      <c r="A43" s="14"/>
+      <c r="A43" s="12"/>
       <c r="B43" s="6"/>
       <c r="C43" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:3">
-      <c r="A44" s="14"/>
+      <c r="A44" s="12"/>
       <c r="B44" s="6"/>
       <c r="C44" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
-      <c r="A45" s="14"/>
+      <c r="A45" s="12"/>
       <c r="B45" s="6"/>
       <c r="C45" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="46" ht="15" spans="1:3">
-      <c r="A46" s="14"/>
+      <c r="A46" s="12"/>
       <c r="B46" s="6"/>
       <c r="C46" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="14"/>
-      <c r="C47" s="15"/>
+      <c r="A47" s="12"/>
+      <c r="C47" s="13"/>
     </row>
     <row r="48" ht="15" spans="1:3">
-      <c r="A48" s="14"/>
+      <c r="A48" s="12"/>
       <c r="B48" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="24" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
-      <c r="A49" s="14"/>
+      <c r="A49" s="12"/>
       <c r="B49" s="6"/>
       <c r="C49" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
-      <c r="A50" s="14"/>
+      <c r="A50" s="12"/>
       <c r="B50" s="6"/>
       <c r="C50" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
-      <c r="A51" s="14"/>
+      <c r="A51" s="12"/>
       <c r="B51" s="6"/>
       <c r="C51" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
-      <c r="A52" s="14"/>
+      <c r="A52" s="12"/>
       <c r="B52" s="6"/>
       <c r="C52" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="53" ht="18" spans="1:3">
-      <c r="A53" s="14"/>
-      <c r="B53" s="26"/>
+      <c r="A53" s="12"/>
+      <c r="B53" s="25"/>
       <c r="C53" s="5"/>
     </row>
     <row r="54" ht="15" spans="1:3">
-      <c r="A54" s="14"/>
+      <c r="A54" s="12"/>
       <c r="B54" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C54" s="25" t="s">
+      <c r="C54" s="24" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="55" ht="15" spans="1:3">
-      <c r="A55" s="14"/>
+      <c r="A55" s="12"/>
       <c r="B55" s="6"/>
       <c r="C55" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="56" ht="15" spans="1:3">
-      <c r="A56" s="14"/>
+      <c r="A56" s="12"/>
       <c r="B56" s="6"/>
       <c r="C56" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="57" ht="15" spans="1:3">
-      <c r="A57" s="14"/>
+      <c r="A57" s="12"/>
       <c r="B57" s="6"/>
       <c r="C57" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="58" ht="15" spans="1:3">
-      <c r="A58" s="14"/>
+      <c r="A58" s="12"/>
       <c r="B58" s="6"/>
       <c r="C58" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="59" ht="15" spans="1:3">
-      <c r="A59" s="14"/>
+      <c r="A59" s="12"/>
       <c r="B59" s="6"/>
       <c r="C59" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="60" ht="15" spans="1:3">
-      <c r="A60" s="14"/>
+      <c r="A60" s="12"/>
       <c r="B60" s="6"/>
       <c r="C60" s="5"/>
     </row>
     <row r="61" ht="15" spans="1:3">
-      <c r="A61" s="14"/>
+      <c r="A61" s="12"/>
       <c r="B61" s="6" t="s">
         <v>71</v>
       </c>
@@ -2984,72 +2993,72 @@
       </c>
     </row>
     <row r="62" ht="15" spans="1:3">
-      <c r="A62" s="14"/>
+      <c r="A62" s="12"/>
       <c r="B62" s="6"/>
       <c r="C62" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="63" ht="15" spans="1:3">
-      <c r="A63" s="14"/>
+      <c r="A63" s="12"/>
       <c r="B63" s="6"/>
       <c r="C63" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="64" ht="15" spans="1:3">
-      <c r="A64" s="14"/>
+      <c r="A64" s="12"/>
       <c r="B64" s="6"/>
       <c r="C64" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="65" ht="15" spans="1:3">
-      <c r="A65" s="14"/>
+      <c r="A65" s="12"/>
       <c r="B65" s="6"/>
       <c r="C65" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="66" ht="15" spans="1:3">
-      <c r="A66" s="14"/>
+      <c r="A66" s="12"/>
       <c r="B66" s="6"/>
       <c r="C66" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="67" ht="15" spans="1:3">
-      <c r="A67" s="14"/>
-      <c r="B67" s="27"/>
+      <c r="A67" s="12"/>
+      <c r="B67" s="26"/>
       <c r="C67" s="5"/>
     </row>
     <row r="68" ht="15" spans="1:3">
-      <c r="A68" s="14"/>
-      <c r="B68" s="4" t="s">
+      <c r="A68" s="12"/>
+      <c r="B68" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="69" ht="15" spans="1:3">
-      <c r="A69" s="14"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="9" t="s">
+      <c r="A69" s="12"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="7" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="14"/>
-      <c r="B70" s="4"/>
+      <c r="A70" s="12"/>
+      <c r="B70" s="14"/>
       <c r="C70" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="71" ht="9" customHeight="1" spans="1:3">
-      <c r="A71" s="10"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
+      <c r="A71" s="8"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3114,7 +3123,7 @@
       <c r="A3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -3122,12 +3131,12 @@
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="5"/>
     </row>
     <row r="5" ht="15" spans="1:3">
-      <c r="A5" s="14"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
         <v>80</v>
       </c>
@@ -3136,40 +3145,40 @@
       </c>
     </row>
     <row r="6" ht="15" spans="1:3">
-      <c r="A6" s="14"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="6"/>
       <c r="C6" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
-      <c r="A7" s="14"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="6"/>
       <c r="C7" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
-      <c r="A8" s="14"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="6"/>
       <c r="C8" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
-      <c r="A9" s="14"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="1:3">
-      <c r="A10" s="14"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="6"/>
       <c r="C10" s="5"/>
     </row>
     <row r="11" ht="15" spans="1:3">
-      <c r="A11" s="14"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="6" t="s">
         <v>85</v>
       </c>
@@ -3178,61 +3187,61 @@
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
-      <c r="A12" s="14"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
-      <c r="A13" s="14"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
-      <c r="A14" s="14"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:3">
-      <c r="A15" s="14"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:3">
-      <c r="A16" s="14"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
-      <c r="A17" s="14"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
-      <c r="A18" s="14"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="19" ht="18.75" spans="1:3">
-      <c r="A19" s="14"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="18"/>
+      <c r="C19" s="17"/>
     </row>
     <row r="20" ht="15" spans="1:3">
-      <c r="A20" s="14"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="6" t="s">
         <v>94</v>
       </c>
@@ -3241,54 +3250,54 @@
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="6"/>
       <c r="C21" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
-      <c r="A22" s="14"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="6"/>
       <c r="C22" s="5" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
-      <c r="A23" s="14"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="6"/>
       <c r="C23" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:3">
-      <c r="A24" s="14"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="6"/>
       <c r="C24" s="5" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
-      <c r="A25" s="14"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="6"/>
       <c r="C25" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="26" ht="15" spans="1:3">
-      <c r="A26" s="14"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="6"/>
       <c r="C26" s="5" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="27" ht="15.75" spans="1:3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="5"/>
     </row>
     <row r="28" ht="15" spans="1:3">
-      <c r="A28" s="14"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="6" t="s">
         <v>101</v>
       </c>
@@ -3297,47 +3306,47 @@
       </c>
     </row>
     <row r="29" ht="15" spans="1:3">
-      <c r="A29" s="14"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="6"/>
       <c r="C29" s="5" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:3">
-      <c r="A30" s="14"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="6"/>
       <c r="C30" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
-      <c r="A31" s="14"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="6"/>
       <c r="C31" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
-      <c r="A32" s="14"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="6"/>
       <c r="C32" s="5" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
-      <c r="A33" s="14"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="6"/>
       <c r="C33" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="34" ht="15" spans="1:3">
-      <c r="A34" s="14"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="15"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" ht="15" spans="1:3">
-      <c r="A35" s="14"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="6" t="s">
         <v>106</v>
       </c>
@@ -3346,61 +3355,61 @@
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
-      <c r="A36" s="14"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="6"/>
       <c r="C36" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="37" ht="15" spans="1:3">
-      <c r="A37" s="14"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="6"/>
       <c r="C37" s="5" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:3">
-      <c r="A38" s="14"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="6"/>
       <c r="C38" s="5" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
-      <c r="A39" s="14"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="6"/>
       <c r="C39" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
-      <c r="A40" s="14"/>
+      <c r="A40" s="12"/>
       <c r="B40" s="6"/>
       <c r="C40" s="5" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="41" ht="15" spans="1:3">
-      <c r="A41" s="14"/>
+      <c r="A41" s="12"/>
       <c r="B41" s="6"/>
       <c r="C41" s="5" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:3">
-      <c r="A42" s="14"/>
+      <c r="A42" s="12"/>
       <c r="B42" s="6"/>
       <c r="C42" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
-      <c r="A43" s="14"/>
-      <c r="B43" s="22"/>
-      <c r="C43" s="15"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="13"/>
     </row>
     <row r="44" ht="15" spans="1:3">
-      <c r="A44" s="14"/>
+      <c r="A44" s="12"/>
       <c r="B44" s="6" t="s">
         <v>113</v>
       </c>
@@ -3409,33 +3418,33 @@
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
-      <c r="A45" s="14"/>
+      <c r="A45" s="12"/>
       <c r="B45" s="6"/>
       <c r="C45" s="5" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="46" ht="15" spans="1:3">
-      <c r="A46" s="14"/>
+      <c r="A46" s="12"/>
       <c r="B46" s="6"/>
       <c r="C46" s="5" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="47" ht="15" spans="1:3">
-      <c r="A47" s="14"/>
+      <c r="A47" s="12"/>
       <c r="B47" s="6"/>
       <c r="C47" s="5" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="48" ht="15" spans="1:3">
-      <c r="A48" s="14"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="15"/>
+      <c r="A48" s="12"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="13"/>
     </row>
     <row r="49" ht="15" spans="1:3">
-      <c r="A49" s="14"/>
+      <c r="A49" s="12"/>
       <c r="B49" s="6" t="s">
         <v>117</v>
       </c>
@@ -3444,40 +3453,40 @@
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
-      <c r="A50" s="14"/>
+      <c r="A50" s="12"/>
       <c r="B50" s="6"/>
       <c r="C50" s="5" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
-      <c r="A51" s="14"/>
+      <c r="A51" s="12"/>
       <c r="B51" s="6"/>
       <c r="C51" s="5" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
-      <c r="A52" s="14"/>
+      <c r="A52" s="12"/>
       <c r="B52" s="6"/>
       <c r="C52" s="5" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
-      <c r="A53" s="14"/>
+      <c r="A53" s="12"/>
       <c r="B53" s="6"/>
       <c r="C53" s="5" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="54" ht="15.75" spans="1:3">
-      <c r="A54" s="14"/>
+      <c r="A54" s="12"/>
       <c r="B54" s="6"/>
       <c r="C54" s="5"/>
     </row>
     <row r="55" ht="33" customHeight="1" spans="1:3">
-      <c r="A55" s="14"/>
+      <c r="A55" s="12"/>
       <c r="B55" s="6" t="s">
         <v>123</v>
       </c>
@@ -3486,67 +3495,67 @@
       </c>
     </row>
     <row r="56" ht="33" customHeight="1" spans="1:3">
-      <c r="A56" s="14"/>
+      <c r="A56" s="12"/>
       <c r="B56" s="6"/>
       <c r="C56" s="5" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="57" ht="33" customHeight="1" spans="1:3">
-      <c r="A57" s="14"/>
+      <c r="A57" s="12"/>
       <c r="B57" s="6"/>
       <c r="C57" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="58" ht="33" customHeight="1" spans="1:3">
-      <c r="A58" s="14"/>
+      <c r="A58" s="12"/>
       <c r="B58" s="6"/>
       <c r="C58" s="5" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="59" ht="33" customHeight="1" spans="1:3">
-      <c r="A59" s="14"/>
+      <c r="A59" s="12"/>
       <c r="B59" s="6"/>
       <c r="C59" s="5" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="60" ht="33" customHeight="1" spans="1:3">
-      <c r="A60" s="14"/>
+      <c r="A60" s="12"/>
       <c r="B60" s="6"/>
       <c r="C60" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="61" ht="15" spans="1:3">
-      <c r="A61" s="14"/>
-      <c r="B61" s="4" t="s">
+      <c r="A61" s="12"/>
+      <c r="B61" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1" spans="1:3">
-      <c r="A62" s="14"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="9" t="s">
+      <c r="A62" s="12"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="63" ht="15" spans="1:3">
-      <c r="A63" s="14"/>
-      <c r="B63" s="4"/>
+      <c r="A63" s="12"/>
+      <c r="B63" s="14"/>
       <c r="C63" s="5" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="64" ht="8" customHeight="1" spans="1:3">
-      <c r="A64" s="10"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3608,7 +3617,7 @@
       <c r="A3" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -3617,7 +3626,7 @@
     </row>
     <row r="4" ht="15.75" spans="1:3">
       <c r="A4" s="3"/>
-      <c r="B4" s="11"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="5"/>
     </row>
     <row r="5" ht="15.75" spans="1:3">
@@ -3660,7 +3669,7 @@
     <row r="10" ht="18.75" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="18"/>
+      <c r="C10" s="17"/>
     </row>
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="3"/>
@@ -3687,7 +3696,7 @@
     </row>
     <row r="14" ht="15.75" spans="1:3">
       <c r="A14" s="3"/>
-      <c r="B14" s="7"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="5"/>
     </row>
     <row r="15" ht="15" spans="1:3">
@@ -3715,8 +3724,8 @@
     </row>
     <row r="18" ht="15" spans="1:3">
       <c r="A18" s="3"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="15"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" ht="15" spans="1:3">
       <c r="A19" s="3"/>
@@ -3743,50 +3752,50 @@
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="3"/>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1" spans="1:3">
       <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="23" t="s">
+      <c r="B23" s="14"/>
+      <c r="C23" s="22" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="23"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="22"/>
     </row>
     <row r="25" ht="13" customHeight="1" spans="1:3">
       <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="8" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="15" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="26" ht="15" spans="1:3">
       <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="23" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="22" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="27" ht="15" spans="1:3">
       <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="23" t="s">
+      <c r="B27" s="14"/>
+      <c r="C27" s="22" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="28" ht="8" customHeight="1" spans="1:3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3841,176 +3850,176 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="18.75" spans="1:3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" ht="15" spans="1:3">
-      <c r="A4" s="19"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
     <row r="5" ht="18.75" spans="1:3">
-      <c r="A5" s="19"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="6" ht="18.75" spans="1:3">
-      <c r="A6" s="19"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="7" ht="18.75" spans="1:3">
-      <c r="A7" s="19"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="8" ht="18.75" spans="1:3">
-      <c r="A8" s="19"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
-      <c r="A9" s="19"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
     <row r="10" ht="18.75" spans="1:3">
-      <c r="A10" s="19"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="11" ht="18.75" spans="1:3">
-      <c r="A11" s="19"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="12" ht="37.5" spans="1:3">
-      <c r="A12" s="19"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="13" ht="18.75" spans="1:3">
-      <c r="A13" s="19"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="14" ht="37.5" spans="1:3">
-      <c r="A14" s="19"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="17" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="15" ht="18.75" spans="1:3">
-      <c r="A15" s="19"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="16" ht="37.5" spans="1:3">
-      <c r="A16" s="19"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="17" ht="18.75" spans="1:3">
-      <c r="A17" s="19"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="18" ht="37.5" spans="1:3">
-      <c r="A18" s="19"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="19" ht="18.75" spans="1:3">
-      <c r="A19" s="19"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="17" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="20" ht="18.75" spans="1:3">
-      <c r="A20" s="19"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="17" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="21" ht="18.75" spans="1:3">
-      <c r="A21" s="19"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="17" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="22" ht="18.75" spans="1:3">
-      <c r="A22" s="19"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="17" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="23" ht="18.75" spans="1:3">
-      <c r="A23" s="19"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="17" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="24" ht="18.75" spans="1:3">
-      <c r="A24" s="19"/>
-      <c r="B24" s="20" t="s">
+      <c r="A24" s="18"/>
+      <c r="B24" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="20" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="25" ht="37.5" spans="1:3">
-      <c r="A25" s="19"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="18" t="s">
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="17" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="26" ht="9" customHeight="1" spans="1:3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4066,7 +4075,7 @@
       <c r="A3" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -4074,12 +4083,12 @@
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="5"/>
     </row>
     <row r="5" ht="15" spans="1:3">
-      <c r="A5" s="14"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
         <v>179</v>
       </c>
@@ -4088,82 +4097,82 @@
       </c>
     </row>
     <row r="6" ht="15" spans="1:3">
-      <c r="A6" s="14"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="6"/>
       <c r="C6" s="5" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
-      <c r="A7" s="14"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="6"/>
       <c r="C7" s="5" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
-      <c r="A8" s="14"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="6"/>
       <c r="C8" s="5" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
-      <c r="A9" s="14"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
-      <c r="A10" s="14"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="6"/>
       <c r="C10" s="5" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:3">
-      <c r="A11" s="14"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
-      <c r="A12" s="14"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
-      <c r="A13" s="14"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="5" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
-      <c r="A14" s="14"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:3">
-      <c r="A15" s="14"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="16" ht="15.75" spans="1:3">
-      <c r="A16" s="14"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5"/>
     </row>
     <row r="17" ht="15" spans="1:3">
-      <c r="A17" s="14"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="6" t="s">
         <v>190</v>
       </c>
@@ -4172,86 +4181,86 @@
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
-      <c r="A18" s="14"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:3">
-      <c r="A19" s="14"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="6"/>
       <c r="C19" s="5" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
-      <c r="A20" s="14"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="6"/>
       <c r="C20" s="5" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="6"/>
       <c r="C21" s="5" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
-      <c r="A22" s="14"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="6"/>
       <c r="C22" s="5" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
-      <c r="A23" s="14"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="6"/>
       <c r="C23" s="5" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:3">
-      <c r="A24" s="14"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="6"/>
       <c r="C24" s="5" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
-      <c r="A25" s="14"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="6"/>
       <c r="C25" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="14"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="15"/>
+      <c r="C26" s="13"/>
     </row>
     <row r="27" ht="15" spans="1:3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="12"/>
+      <c r="B27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1" spans="1:3">
-      <c r="A28" s="14"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="9" t="s">
+      <c r="A28" s="12"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="7" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="29" ht="8" customHeight="1" spans="1:3">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
     </row>
     <row r="30" customFormat="1" ht="24.75" spans="1:3">
       <c r="A30" s="2" t="s">
@@ -4261,7 +4270,7 @@
       <c r="C30" s="2"/>
     </row>
     <row r="31" ht="15" spans="1:3">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="10" t="s">
         <v>201</v>
       </c>
       <c r="B31" s="6" t="s">
@@ -4272,75 +4281,75 @@
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
-      <c r="A32" s="12"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="6"/>
       <c r="C32" s="5" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
-      <c r="A33" s="12"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="6"/>
       <c r="C33" s="5" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="34" ht="15" spans="1:3">
-      <c r="A34" s="12"/>
+      <c r="A34" s="10"/>
       <c r="B34" s="6"/>
       <c r="C34" s="5" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:3">
-      <c r="A35" s="12"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="6"/>
       <c r="C35" s="5" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
-      <c r="A36" s="12"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="6"/>
       <c r="C36" s="5" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="37" ht="15" spans="1:3">
-      <c r="A37" s="12"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="6"/>
       <c r="C37" s="5" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:3">
-      <c r="A38" s="12"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="6"/>
       <c r="C38" s="5" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
-      <c r="A39" s="12"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="6"/>
       <c r="C39" s="5" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
-      <c r="A40" s="12"/>
+      <c r="A40" s="10"/>
       <c r="B40" s="6"/>
       <c r="C40" s="5" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="41" ht="15.75" spans="1:3">
-      <c r="A41" s="12"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="9"/>
       <c r="C41" s="5"/>
     </row>
     <row r="42" ht="15" spans="1:3">
-      <c r="A42" s="12"/>
+      <c r="A42" s="10"/>
       <c r="B42" s="6" t="s">
         <v>212</v>
       </c>
@@ -4349,102 +4358,102 @@
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
-      <c r="A43" s="12"/>
+      <c r="A43" s="10"/>
       <c r="B43" s="6"/>
       <c r="C43" s="5" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:3">
-      <c r="A44" s="12"/>
+      <c r="A44" s="10"/>
       <c r="B44" s="6"/>
       <c r="C44" s="5" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
-      <c r="A45" s="12"/>
+      <c r="A45" s="10"/>
       <c r="B45" s="6"/>
       <c r="C45" s="5" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="46" ht="15" spans="1:3">
-      <c r="A46" s="12"/>
+      <c r="A46" s="10"/>
       <c r="B46" s="6"/>
       <c r="C46" s="5" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="47" ht="15" spans="1:3">
-      <c r="A47" s="12"/>
+      <c r="A47" s="10"/>
       <c r="B47" s="6"/>
       <c r="C47" s="5" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="48" ht="15" spans="1:3">
-      <c r="A48" s="12"/>
+      <c r="A48" s="10"/>
       <c r="B48" s="6"/>
       <c r="C48" s="5" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
-      <c r="A49" s="12"/>
+      <c r="A49" s="10"/>
       <c r="B49" s="6"/>
       <c r="C49" s="5" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
-      <c r="A50" s="12"/>
+      <c r="A50" s="10"/>
       <c r="B50" s="6"/>
       <c r="C50" s="5" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="12"/>
+      <c r="A51" s="10"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="13" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="12"/>
+      <c r="A52" s="10"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="13" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="12"/>
+      <c r="A53" s="10"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="15" t="s">
+      <c r="C53" s="13" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="54" ht="15" spans="1:3">
-      <c r="A54" s="12"/>
-      <c r="B54" s="4" t="s">
+      <c r="A54" s="10"/>
+      <c r="B54" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="55" ht="15" spans="1:3">
-      <c r="A55" s="12"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="16" t="s">
+      <c r="A55" s="10"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="7" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="56" customFormat="1" ht="9" customHeight="1" spans="1:3">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
     </row>
     <row r="57" ht="18.75" spans="1:1">
       <c r="A57" s="3"/>
@@ -4548,12 +4557,12 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="3"/>
@@ -4586,7 +4595,7 @@
       <c r="A3" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -4595,7 +4604,7 @@
     </row>
     <row r="4" ht="15.75" spans="1:3">
       <c r="A4" s="3"/>
-      <c r="B4" s="11"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="5"/>
     </row>
     <row r="5" ht="15" spans="1:3">
@@ -4726,7 +4735,7 @@
     </row>
     <row r="23" ht="15.75" spans="1:3">
       <c r="A23" s="3"/>
-      <c r="B23" s="7"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="5"/>
     </row>
     <row r="24" ht="15" spans="1:3">
@@ -4794,241 +4803,206 @@
         <v>253</v>
       </c>
     </row>
-    <row r="33" ht="15" spans="1:3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" ht="15" spans="1:3">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="9" t="s">
+    <row r="33" customFormat="1" ht="9" customHeight="1" spans="1:3">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" customFormat="1" ht="24.75" spans="1:3">
+      <c r="A34" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="35" customFormat="1" ht="9" customHeight="1" spans="1:3">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-    </row>
-    <row r="36" customFormat="1" ht="24.75" spans="1:3">
-      <c r="A36" s="2" t="s">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" ht="15" spans="1:3">
+      <c r="A35" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="B35" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="36" ht="15" spans="1:3">
+      <c r="A36" s="10"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="5" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="37" ht="15" spans="1:3">
-      <c r="A37" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>257</v>
-      </c>
+      <c r="A37" s="10"/>
+      <c r="B37" s="6"/>
       <c r="C37" s="5" t="s">
-        <v>232</v>
+        <v>258</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:3">
-      <c r="A38" s="12"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="6"/>
       <c r="C38" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
-      <c r="A39" s="12"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="6"/>
       <c r="C39" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
-      <c r="A40" s="12"/>
+      <c r="A40" s="10"/>
       <c r="B40" s="6"/>
       <c r="C40" s="5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="41" ht="15" spans="1:3">
-      <c r="A41" s="12"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="5" t="s">
         <v>261</v>
       </c>
     </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="10"/>
+    </row>
     <row r="42" ht="15" spans="1:3">
-      <c r="A42" s="12"/>
-      <c r="B42" s="6"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="6" t="s">
+        <v>262</v>
+      </c>
       <c r="C42" s="5" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="12"/>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="43" ht="15" spans="1:3">
+      <c r="A43" s="10"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="5" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="44" ht="15" spans="1:3">
-      <c r="A44" s="12"/>
-      <c r="B44" s="6" t="s">
-        <v>263</v>
-      </c>
+      <c r="A44" s="10"/>
+      <c r="B44" s="6"/>
       <c r="C44" s="5" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
-      <c r="A45" s="12"/>
+      <c r="A45" s="10"/>
       <c r="B45" s="6"/>
       <c r="C45" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46" ht="15" spans="1:3">
-      <c r="A46" s="12"/>
+      <c r="A46" s="10"/>
       <c r="B46" s="6"/>
       <c r="C46" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="47" ht="15" spans="1:3">
-      <c r="A47" s="12"/>
+      <c r="A47" s="10"/>
       <c r="B47" s="6"/>
       <c r="C47" s="5" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="48" ht="15" spans="1:3">
-      <c r="A48" s="12"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="5" t="s">
         <v>267</v>
       </c>
     </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="10"/>
+    </row>
     <row r="49" ht="15" spans="1:3">
-      <c r="A49" s="12"/>
-      <c r="B49" s="6"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="6" t="s">
+        <v>268</v>
+      </c>
       <c r="C49" s="5" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="12"/>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="50" ht="15" spans="1:3">
+      <c r="A50" s="10"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="5" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="51" ht="15" spans="1:3">
-      <c r="A51" s="12"/>
-      <c r="B51" s="6" t="s">
-        <v>269</v>
-      </c>
+      <c r="A51" s="10"/>
+      <c r="B51" s="6"/>
       <c r="C51" s="5" t="s">
-        <v>232</v>
+        <v>270</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
-      <c r="A52" s="12"/>
+      <c r="A52" s="10"/>
       <c r="B52" s="6"/>
       <c r="C52" s="5" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="53" ht="15" spans="1:3">
-      <c r="A53" s="12"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="5" t="s">
         <v>271</v>
       </c>
     </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="10"/>
+    </row>
     <row r="54" ht="15" spans="1:3">
-      <c r="A54" s="12"/>
-      <c r="B54" s="6"/>
+      <c r="A54" s="10"/>
+      <c r="B54" s="6" t="s">
+        <v>272</v>
+      </c>
       <c r="C54" s="5" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="12"/>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="55" ht="15" spans="1:3">
+      <c r="A55" s="10"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="5" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="56" ht="15" spans="1:3">
-      <c r="A56" s="12"/>
-      <c r="B56" s="6" t="s">
-        <v>273</v>
-      </c>
+      <c r="A56" s="10"/>
+      <c r="B56" s="6"/>
       <c r="C56" s="5" t="s">
-        <v>232</v>
+        <v>274</v>
       </c>
     </row>
     <row r="57" ht="15" spans="1:3">
-      <c r="A57" s="12"/>
+      <c r="A57" s="10"/>
       <c r="B57" s="6"/>
       <c r="C57" s="5" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="58" ht="15" spans="1:3">
-      <c r="A58" s="12"/>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="10"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="5" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="59" ht="15" spans="1:3">
-      <c r="A59" s="12"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="5" t="s">
+      <c r="C58" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="12"/>
-      <c r="B60" s="6"/>
-      <c r="C60" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="61" ht="18.75" spans="1:3">
-      <c r="A61" s="12"/>
-      <c r="B61" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" ht="18.75" spans="1:3">
-      <c r="A62" s="12"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="9" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="10"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-    </row>
-    <row r="72" ht="44.25" spans="4:4">
-      <c r="D72" s="13"/>
+    <row r="59" spans="1:3">
+      <c r="A59" s="8"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+    </row>
+    <row r="68" ht="44.25" spans="4:4">
+      <c r="D68" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="12">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A3:A34"/>
-    <mergeCell ref="A37:A60"/>
-    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A3:A32"/>
+    <mergeCell ref="A35:A58"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B15:B22"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B35:B40"/>
+    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="B54:B58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -5038,12 +5012,12 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -5067,160 +5041,185 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" ht="15" spans="1:3">
+    <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>281</v>
+        <v>23</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="4" ht="15" spans="1:3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:3">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
-        <v>282</v>
-      </c>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
+      <c r="B5" s="6" t="s">
+        <v>279</v>
+      </c>
       <c r="C5" s="5" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:3">
       <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="5" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="10" ht="15" spans="1:3">
       <c r="A10" s="3"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="3"/>
-      <c r="B11" s="6" t="s">
-        <v>288</v>
-      </c>
+      <c r="B11" s="6"/>
       <c r="C11" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="12" ht="15" spans="1:3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
       <c r="A12" s="3"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="13" ht="15" spans="1:3">
       <c r="A13" s="3"/>
-      <c r="B13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>287</v>
+      </c>
       <c r="C13" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
       <c r="A14" s="3"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:3">
       <c r="A16" s="3"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="3"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" spans="1:3">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="19" ht="15" spans="1:3">
       <c r="A19" s="3"/>
-      <c r="B19" s="7"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="3"/>
-      <c r="B20" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" ht="30" spans="1:3">
+      <c r="B20" s="6"/>
+      <c r="C20" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" spans="1:3">
       <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="9" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" ht="15" spans="1:3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="5" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="22" customFormat="1" ht="9" customHeight="1" spans="1:3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
+    <row r="23" ht="15" spans="1:3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="24" ht="15" spans="1:3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="6"/>
+      <c r="C25" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" customFormat="1" ht="9" customHeight="1" spans="1:3">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:A21"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="B11:B18"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A3:A25"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="B13:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>